<commit_message>
0809 var-diameter exp completed
</commit_message>
<xml_diff>
--- a/PycharmCodes_xlsxFiles/var_diam_data18mm.xlsx
+++ b/PycharmCodes_xlsxFiles/var_diam_data18mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d89e7b822021c56/Documents/성균관대학교/LAB/skku_robotory/PycharmCodes_xlsxFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="8_{07F248D2-7856-40A1-9CC6-E90616BB21F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46A77F0D-D360-4B43-BA10-9E30E1157835}"/>
+  <xr:revisionPtr revIDLastSave="506" documentId="8_{07F248D2-7856-40A1-9CC6-E90616BB21F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CC89298-BC55-419F-A839-FD3207399554}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{A802EB2F-1C16-4A1A-977F-EE60EBC50092}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A802EB2F-1C16-4A1A-977F-EE60EBC50092}"/>
   </bookViews>
   <sheets>
     <sheet name="dn" sheetId="1" r:id="rId1"/>
@@ -300,7 +300,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +363,22 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -386,7 +402,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -406,6 +422,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -748,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC1814F-43B7-4DF4-857A-25F58CC7AECE}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -829,6 +851,15 @@
       <c r="D2" s="4">
         <v>0.68</v>
       </c>
+      <c r="E2" s="6">
+        <v>1.28</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.96</v>
+      </c>
       <c r="H2" s="3">
         <v>1.25</v>
       </c>
@@ -838,6 +869,15 @@
       <c r="J2" s="3">
         <v>1.31</v>
       </c>
+      <c r="K2" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="L2" s="6">
+        <v>1.47</v>
+      </c>
+      <c r="M2" s="6">
+        <v>1.48</v>
+      </c>
       <c r="N2" s="3">
         <v>2.16</v>
       </c>
@@ -846,6 +886,15 @@
       </c>
       <c r="P2" s="3">
         <v>2.09</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>4.45</v>
+      </c>
+      <c r="R2" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="S2" s="6">
+        <v>4.34</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
@@ -861,6 +910,15 @@
       <c r="D3" s="4">
         <v>1.06</v>
       </c>
+      <c r="E3" s="6">
+        <v>2.11</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1.86</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1.89</v>
+      </c>
       <c r="H3" s="3">
         <v>2.52</v>
       </c>
@@ -870,6 +928,15 @@
       <c r="J3" s="3">
         <v>2.5499999999999998</v>
       </c>
+      <c r="K3" s="6">
+        <v>2.64</v>
+      </c>
+      <c r="L3" s="6">
+        <v>2.58</v>
+      </c>
+      <c r="M3" s="6">
+        <v>2.94</v>
+      </c>
       <c r="N3" s="3">
         <v>4.1900000000000004</v>
       </c>
@@ -878,6 +945,15 @@
       </c>
       <c r="P3" s="3">
         <v>3.99</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>5.94</v>
+      </c>
+      <c r="R3" s="6">
+        <v>5.71</v>
+      </c>
+      <c r="S3" s="6">
+        <v>5.88</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
@@ -893,6 +969,15 @@
       <c r="D4" s="4">
         <v>1.47</v>
       </c>
+      <c r="E4" s="6">
+        <v>2.82</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2.78</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2.82</v>
+      </c>
       <c r="H4" s="3">
         <v>3.65</v>
       </c>
@@ -902,6 +987,15 @@
       <c r="J4" s="3">
         <v>3.69</v>
       </c>
+      <c r="K4" s="6">
+        <v>4.26</v>
+      </c>
+      <c r="L4" s="6">
+        <v>4.68</v>
+      </c>
+      <c r="M4" s="6">
+        <v>4.6399999999999997</v>
+      </c>
       <c r="N4" s="3">
         <v>6.11</v>
       </c>
@@ -910,6 +1004,15 @@
       </c>
       <c r="P4" s="3">
         <v>5.83</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>7.4</v>
+      </c>
+      <c r="R4" s="6">
+        <v>7.18</v>
+      </c>
+      <c r="S4" s="6">
+        <v>6.97</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
@@ -925,6 +1028,15 @@
       <c r="D5" s="4">
         <v>1.8</v>
       </c>
+      <c r="E5" s="6">
+        <v>3.55</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3.57</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3.59</v>
+      </c>
       <c r="H5" s="3">
         <v>4.6500000000000004</v>
       </c>
@@ -934,6 +1046,15 @@
       <c r="J5" s="3">
         <v>4.74</v>
       </c>
+      <c r="K5" s="6">
+        <v>5.51</v>
+      </c>
+      <c r="L5" s="6">
+        <v>5.61</v>
+      </c>
+      <c r="M5" s="6">
+        <v>5.68</v>
+      </c>
       <c r="N5" s="3">
         <v>7.6</v>
       </c>
@@ -942,6 +1063,15 @@
       </c>
       <c r="P5" s="3">
         <v>7.55</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>8.85</v>
+      </c>
+      <c r="R5" s="6">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="S5" s="6">
+        <v>8.4700000000000006</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
@@ -957,6 +1087,15 @@
       <c r="D6" s="4">
         <v>2.12</v>
       </c>
+      <c r="E6" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4.29</v>
+      </c>
+      <c r="G6" s="6">
+        <v>4.3099999999999996</v>
+      </c>
       <c r="H6" s="3">
         <v>5.61</v>
       </c>
@@ -966,6 +1105,15 @@
       <c r="J6" s="3">
         <v>5.69</v>
       </c>
+      <c r="K6" s="6">
+        <v>6.74</v>
+      </c>
+      <c r="L6" s="6">
+        <v>6.26</v>
+      </c>
+      <c r="M6" s="6">
+        <v>6.22</v>
+      </c>
       <c r="N6" s="3">
         <v>8.9499999999999993</v>
       </c>
@@ -974,6 +1122,15 @@
       </c>
       <c r="P6" s="3">
         <v>9.15</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>10.53</v>
+      </c>
+      <c r="R6" s="6">
+        <v>10.08</v>
+      </c>
+      <c r="S6" s="6">
+        <v>10.29</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
@@ -996,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2962F089-5977-4595-9196-419C29712554}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1072,6 +1229,15 @@
       <c r="D2" s="4">
         <v>0.3</v>
       </c>
+      <c r="E2" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.48</v>
+      </c>
       <c r="H2" s="3">
         <v>0.98</v>
       </c>
@@ -1081,6 +1247,15 @@
       <c r="J2" s="3">
         <v>0.89</v>
       </c>
+      <c r="K2" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="L2" s="8">
+        <v>1.44</v>
+      </c>
+      <c r="M2" s="8">
+        <v>1.22</v>
+      </c>
       <c r="N2" s="3">
         <v>1.66</v>
       </c>
@@ -1089,6 +1264,15 @@
       </c>
       <c r="P2" s="3">
         <v>1.55</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="R2" s="8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="S2" s="8">
+        <v>2.48</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
@@ -1104,6 +1288,15 @@
       <c r="D3" s="4">
         <v>1.22</v>
       </c>
+      <c r="E3" s="8">
+        <v>1.26</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1.35</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1.32</v>
+      </c>
       <c r="H3" s="3">
         <v>2.21</v>
       </c>
@@ -1113,6 +1306,15 @@
       <c r="J3" s="3">
         <v>2.2000000000000002</v>
       </c>
+      <c r="K3" s="8">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="L3" s="8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="M3" s="8">
+        <v>2.5299999999999998</v>
+      </c>
       <c r="N3" s="3">
         <v>4.46</v>
       </c>
@@ -1121,6 +1323,15 @@
       </c>
       <c r="P3" s="3">
         <v>4.76</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>6.11</v>
+      </c>
+      <c r="R3" s="8">
+        <v>6.13</v>
+      </c>
+      <c r="S3" s="8">
+        <v>6.19</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
@@ -1136,6 +1347,15 @@
       <c r="D4" s="4">
         <v>2.08</v>
       </c>
+      <c r="E4" s="8">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="F4" s="8">
+        <v>2.46</v>
+      </c>
+      <c r="G4" s="8">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="H4" s="3">
         <v>3.32</v>
       </c>
@@ -1145,6 +1365,15 @@
       <c r="J4" s="3">
         <v>3.43</v>
       </c>
+      <c r="K4" s="8">
+        <v>4.83</v>
+      </c>
+      <c r="L4" s="8">
+        <v>4.68</v>
+      </c>
+      <c r="M4" s="8">
+        <v>4.6399999999999997</v>
+      </c>
       <c r="N4" s="3">
         <v>7.51</v>
       </c>
@@ -1153,6 +1382,15 @@
       </c>
       <c r="P4" s="3">
         <v>7.85</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>9.66</v>
+      </c>
+      <c r="R4" s="8">
+        <v>9.65</v>
+      </c>
+      <c r="S4" s="8">
+        <v>9.68</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
@@ -1168,6 +1406,15 @@
       <c r="D5" s="4">
         <v>3.41</v>
       </c>
+      <c r="E5" s="8">
+        <v>3.75</v>
+      </c>
+      <c r="F5" s="8">
+        <v>3.65</v>
+      </c>
+      <c r="G5" s="8">
+        <v>3.57</v>
+      </c>
       <c r="H5" s="3">
         <v>4.51</v>
       </c>
@@ -1177,6 +1424,15 @@
       <c r="J5" s="3">
         <v>5.05</v>
       </c>
+      <c r="K5" s="8">
+        <v>6.7</v>
+      </c>
+      <c r="L5" s="8">
+        <v>6.63</v>
+      </c>
+      <c r="M5" s="8">
+        <v>6.7</v>
+      </c>
       <c r="N5" s="3">
         <v>10.39</v>
       </c>
@@ -1185,6 +1441,15 @@
       </c>
       <c r="P5" s="3">
         <v>10.51</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>13.18</v>
+      </c>
+      <c r="R5" s="8">
+        <v>13.46</v>
+      </c>
+      <c r="S5" s="8">
+        <v>12.95</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
@@ -1200,6 +1465,15 @@
       <c r="D6" s="4">
         <v>4.29</v>
       </c>
+      <c r="E6" s="8">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F6" s="8">
+        <v>4.75</v>
+      </c>
+      <c r="G6" s="8">
+        <v>4.8499999999999996</v>
+      </c>
       <c r="H6" s="3">
         <v>6.21</v>
       </c>
@@ -1209,6 +1483,15 @@
       <c r="J6" s="3">
         <v>6.61</v>
       </c>
+      <c r="K6" s="8">
+        <v>8.61</v>
+      </c>
+      <c r="L6" s="8">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="M6" s="8">
+        <v>8.24</v>
+      </c>
       <c r="N6" s="3">
         <v>13.1</v>
       </c>
@@ -1217,6 +1500,15 @@
       </c>
       <c r="P6" s="3">
         <v>12.98</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>16.95</v>
+      </c>
+      <c r="R6" s="8">
+        <v>17.03</v>
+      </c>
+      <c r="S6" s="8">
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
@@ -1239,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27E905B-DD1C-4250-99B7-1AD1A78A3BED}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1315,6 +1607,15 @@
       <c r="D2" s="4">
         <v>0.56999999999999995</v>
       </c>
+      <c r="E2" s="8">
+        <v>1.52</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1.54</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1.55</v>
+      </c>
       <c r="H2" s="3">
         <v>2.2999999999999998</v>
       </c>
@@ -1324,6 +1625,15 @@
       <c r="J2" s="3">
         <v>2.37</v>
       </c>
+      <c r="K2" s="8">
+        <v>2.85</v>
+      </c>
+      <c r="L2" s="8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="M2" s="8">
+        <v>2.58</v>
+      </c>
       <c r="N2" s="3">
         <v>4.2699999999999996</v>
       </c>
@@ -1332,6 +1642,15 @@
       </c>
       <c r="P2" s="3">
         <v>4.28</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>5.15</v>
+      </c>
+      <c r="R2" s="8">
+        <v>5.61</v>
+      </c>
+      <c r="S2" s="8">
+        <v>5.7</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
@@ -1347,6 +1666,15 @@
       <c r="D3" s="4">
         <v>1.24</v>
       </c>
+      <c r="E3" s="8">
+        <v>3.15</v>
+      </c>
+      <c r="F3" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>4.16</v>
+      </c>
       <c r="H3" s="3">
         <v>4.6900000000000004</v>
       </c>
@@ -1356,6 +1684,15 @@
       <c r="J3" s="3">
         <v>4.62</v>
       </c>
+      <c r="K3" s="8">
+        <v>5.4</v>
+      </c>
+      <c r="L3" s="8">
+        <v>5.86</v>
+      </c>
+      <c r="M3" s="8">
+        <v>5.97</v>
+      </c>
       <c r="N3" s="3">
         <v>8.44</v>
       </c>
@@ -1364,6 +1701,15 @@
       </c>
       <c r="P3" s="3">
         <v>8.49</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>10.52</v>
+      </c>
+      <c r="R3" s="8">
+        <v>10.79</v>
+      </c>
+      <c r="S3" s="8">
+        <v>10.86</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
@@ -1379,6 +1725,15 @@
       <c r="D4" s="4">
         <v>1.97</v>
       </c>
+      <c r="E4" s="8">
+        <v>4.78</v>
+      </c>
+      <c r="F4" s="8">
+        <v>4.79</v>
+      </c>
+      <c r="G4" s="8">
+        <v>4.7699999999999996</v>
+      </c>
       <c r="H4" s="3">
         <v>7.09</v>
       </c>
@@ -1388,6 +1743,15 @@
       <c r="J4" s="3">
         <v>6.92</v>
       </c>
+      <c r="K4" s="8">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L4" s="8">
+        <v>9.31</v>
+      </c>
+      <c r="M4" s="8">
+        <v>8.9499999999999993</v>
+      </c>
       <c r="N4" s="3">
         <v>12.69</v>
       </c>
@@ -1396,6 +1760,15 @@
       </c>
       <c r="P4" s="3">
         <v>12.58</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>15.86</v>
+      </c>
+      <c r="R4" s="8">
+        <v>16.010000000000002</v>
+      </c>
+      <c r="S4" s="8">
+        <v>15.97</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
@@ -1411,6 +1784,15 @@
       <c r="D5" s="4">
         <v>2.76</v>
       </c>
+      <c r="E5" s="8">
+        <v>6.54</v>
+      </c>
+      <c r="F5" s="8">
+        <v>6.49</v>
+      </c>
+      <c r="G5" s="8">
+        <v>6.55</v>
+      </c>
       <c r="H5" s="3">
         <v>9.52</v>
       </c>
@@ -1420,6 +1802,15 @@
       <c r="J5" s="3">
         <v>9.26</v>
       </c>
+      <c r="K5" s="8">
+        <v>12.45</v>
+      </c>
+      <c r="L5" s="8">
+        <v>12.92</v>
+      </c>
+      <c r="M5" s="8">
+        <v>13.01</v>
+      </c>
       <c r="N5" s="3">
         <v>17</v>
       </c>
@@ -1428,6 +1819,15 @@
       </c>
       <c r="P5" s="3">
         <v>17.05</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>21.12</v>
+      </c>
+      <c r="R5" s="8">
+        <v>21.12</v>
+      </c>
+      <c r="S5" s="8">
+        <v>21.06</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
@@ -1443,6 +1843,15 @@
       <c r="D6" s="4">
         <v>3.58</v>
       </c>
+      <c r="E6" s="8">
+        <v>8.32</v>
+      </c>
+      <c r="F6" s="8">
+        <v>8.31</v>
+      </c>
+      <c r="G6" s="8">
+        <v>8.27</v>
+      </c>
       <c r="H6" s="3">
         <v>11.88</v>
       </c>
@@ -1452,6 +1861,15 @@
       <c r="J6" s="3">
         <v>11.59</v>
       </c>
+      <c r="K6" s="8">
+        <v>16.21</v>
+      </c>
+      <c r="L6" s="8">
+        <v>16.54</v>
+      </c>
+      <c r="M6" s="8">
+        <v>16.579999999999998</v>
+      </c>
       <c r="N6" s="3">
         <v>21.13</v>
       </c>
@@ -1460,6 +1878,15 @@
       </c>
       <c r="P6" s="3">
         <v>20.92</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>26.28</v>
+      </c>
+      <c r="R6" s="8">
+        <v>26.13</v>
+      </c>
+      <c r="S6" s="8">
+        <v>26.11</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
@@ -1475,6 +1902,15 @@
       <c r="D7" s="4">
         <v>4.5199999999999996</v>
       </c>
+      <c r="E7" s="8">
+        <v>10.17</v>
+      </c>
+      <c r="F7" s="8">
+        <v>10.08</v>
+      </c>
+      <c r="G7" s="8">
+        <v>10.06</v>
+      </c>
       <c r="H7" s="3">
         <v>14.01</v>
       </c>
@@ -1484,6 +1920,15 @@
       <c r="J7" s="3">
         <v>13.87</v>
       </c>
+      <c r="K7" s="8">
+        <v>19.940000000000001</v>
+      </c>
+      <c r="L7" s="8">
+        <v>20.09</v>
+      </c>
+      <c r="M7" s="8">
+        <v>19.98</v>
+      </c>
       <c r="N7" s="3">
         <v>25.28</v>
       </c>
@@ -1492,6 +1937,15 @@
       </c>
       <c r="P7" s="3">
         <v>25.1</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>31.24</v>
+      </c>
+      <c r="R7" s="8">
+        <v>31.14</v>
+      </c>
+      <c r="S7" s="8">
+        <v>31.24</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
@@ -1507,6 +1961,15 @@
       <c r="D8" s="4">
         <v>5.87</v>
       </c>
+      <c r="E8" s="8">
+        <v>11.92</v>
+      </c>
+      <c r="F8" s="8">
+        <v>11.86</v>
+      </c>
+      <c r="G8" s="8">
+        <v>11.84</v>
+      </c>
       <c r="H8" s="3">
         <v>16.37</v>
       </c>
@@ -1516,6 +1979,15 @@
       <c r="J8" s="3">
         <v>16.149999999999999</v>
       </c>
+      <c r="K8" s="8">
+        <v>23.37</v>
+      </c>
+      <c r="L8" s="8">
+        <v>23.47</v>
+      </c>
+      <c r="M8" s="8">
+        <v>23.24</v>
+      </c>
       <c r="N8" s="3">
         <v>29.16</v>
       </c>
@@ -1524,6 +1996,15 @@
       </c>
       <c r="P8" s="3">
         <v>29.12</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>35.86</v>
+      </c>
+      <c r="R8" s="8">
+        <v>35.76</v>
+      </c>
+      <c r="S8" s="8">
+        <v>35.58</v>
       </c>
     </row>
   </sheetData>
@@ -1536,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705D7C1C-535D-43D9-95F2-A519C4A83F6B}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1559,13 +2040,13 @@
       <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>72</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -1618,6 +2099,15 @@
       <c r="D2" s="4">
         <v>0.26</v>
       </c>
+      <c r="E2" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.89</v>
+      </c>
       <c r="H2" s="3">
         <v>1.1599999999999999</v>
       </c>
@@ -1627,6 +2117,15 @@
       <c r="J2" s="3">
         <v>1.17</v>
       </c>
+      <c r="K2" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="L2" s="8">
+        <v>1.48</v>
+      </c>
+      <c r="M2" s="8">
+        <v>1.46</v>
+      </c>
       <c r="N2" s="3">
         <v>1.45</v>
       </c>
@@ -1635,6 +2134,15 @@
       </c>
       <c r="P2" s="4">
         <v>1.64</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>1.9</v>
+      </c>
+      <c r="R2" s="8">
+        <v>2.06</v>
+      </c>
+      <c r="S2" s="8">
+        <v>2.12</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
@@ -1650,6 +2158,15 @@
       <c r="D3" s="4">
         <v>0.47</v>
       </c>
+      <c r="E3" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1.18</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1.29</v>
+      </c>
       <c r="H3" s="3">
         <v>2.02</v>
       </c>
@@ -1659,6 +2176,15 @@
       <c r="J3" s="3">
         <v>2.0499999999999998</v>
       </c>
+      <c r="K3" s="8">
+        <v>2.27</v>
+      </c>
+      <c r="L3" s="8">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="M3" s="8">
+        <v>2.44</v>
+      </c>
       <c r="N3" s="3">
         <v>2.82</v>
       </c>
@@ -1667,6 +2193,15 @@
       </c>
       <c r="P3" s="3">
         <v>2.92</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>3.65</v>
+      </c>
+      <c r="R3" s="8">
+        <v>3.76</v>
+      </c>
+      <c r="S3" s="8">
+        <v>3.82</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
@@ -1682,6 +2217,15 @@
       <c r="D4" s="4">
         <v>0.67</v>
       </c>
+      <c r="E4" s="8">
+        <v>1.43</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1.59</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1.69</v>
+      </c>
       <c r="H4" s="3">
         <v>2.86</v>
       </c>
@@ -1691,6 +2235,15 @@
       <c r="J4" s="3">
         <v>2.88</v>
       </c>
+      <c r="K4" s="8">
+        <v>3.55</v>
+      </c>
+      <c r="L4" s="8">
+        <v>3.31</v>
+      </c>
+      <c r="M4" s="8">
+        <v>3.45</v>
+      </c>
       <c r="N4" s="3">
         <v>4.1900000000000004</v>
       </c>
@@ -1699,6 +2252,15 @@
       </c>
       <c r="P4" s="3">
         <v>4.3</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>5.36</v>
+      </c>
+      <c r="R4" s="8">
+        <v>5.47</v>
+      </c>
+      <c r="S4" s="8">
+        <v>5.47</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
@@ -1714,6 +2276,15 @@
       <c r="D5" s="4">
         <v>0.88</v>
       </c>
+      <c r="E5" s="8">
+        <v>1.87</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2.1</v>
+      </c>
       <c r="H5" s="3">
         <v>3.69</v>
       </c>
@@ -1723,6 +2294,15 @@
       <c r="J5" s="3">
         <v>3.77</v>
       </c>
+      <c r="K5" s="8">
+        <v>4.38</v>
+      </c>
+      <c r="L5" s="8">
+        <v>4.45</v>
+      </c>
+      <c r="M5" s="8">
+        <v>4.34</v>
+      </c>
       <c r="N5" s="3">
         <v>5.58</v>
       </c>
@@ -1731,6 +2311,15 @@
       </c>
       <c r="P5" s="3">
         <v>5.68</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>7.06</v>
+      </c>
+      <c r="R5" s="8">
+        <v>7.17</v>
+      </c>
+      <c r="S5" s="8">
+        <v>7.19</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
@@ -1746,6 +2335,15 @@
       <c r="D6" s="4">
         <v>1.07</v>
       </c>
+      <c r="E6" s="8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2.42</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2.5</v>
+      </c>
       <c r="H6" s="3">
         <v>4.5</v>
       </c>
@@ -1755,6 +2353,15 @@
       <c r="J6" s="3">
         <v>4.6100000000000003</v>
       </c>
+      <c r="K6" s="8">
+        <v>5.38</v>
+      </c>
+      <c r="L6" s="8">
+        <v>5.29</v>
+      </c>
+      <c r="M6" s="8">
+        <v>5.39</v>
+      </c>
       <c r="N6" s="3">
         <v>6.95</v>
       </c>
@@ -1763,6 +2370,15 @@
       </c>
       <c r="P6" s="3">
         <v>7.04</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>8.68</v>
+      </c>
+      <c r="R6" s="8">
+        <v>8.86</v>
+      </c>
+      <c r="S6" s="8">
+        <v>8.75</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
@@ -1778,6 +2394,15 @@
       <c r="D7" s="4">
         <v>1.27</v>
       </c>
+      <c r="E7" s="8">
+        <v>2.74</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2.85</v>
+      </c>
+      <c r="G7" s="8">
+        <v>2.92</v>
+      </c>
       <c r="H7" s="3">
         <v>5.31</v>
       </c>
@@ -1787,6 +2412,15 @@
       <c r="J7" s="3">
         <v>5.33</v>
       </c>
+      <c r="K7" s="8">
+        <v>6.33</v>
+      </c>
+      <c r="L7" s="8">
+        <v>6.2</v>
+      </c>
+      <c r="M7" s="8">
+        <v>6.29</v>
+      </c>
       <c r="N7" s="3">
         <v>8.3699999999999992</v>
       </c>
@@ -1795,6 +2429,15 @@
       </c>
       <c r="P7" s="3">
         <v>8.43</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>10.26</v>
+      </c>
+      <c r="R7" s="8">
+        <v>10.39</v>
+      </c>
+      <c r="S7" s="8">
+        <v>10.33</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
@@ -1810,6 +2453,15 @@
       <c r="D8" s="4">
         <v>1.47</v>
       </c>
+      <c r="E8" s="8">
+        <v>3.18</v>
+      </c>
+      <c r="F8" s="8">
+        <v>3.27</v>
+      </c>
+      <c r="G8" s="8">
+        <v>3.37</v>
+      </c>
       <c r="H8" s="3">
         <v>6.13</v>
       </c>
@@ -1819,6 +2471,15 @@
       <c r="J8" s="3">
         <v>6.22</v>
       </c>
+      <c r="K8" s="8">
+        <v>7.11</v>
+      </c>
+      <c r="L8" s="8">
+        <v>6.93</v>
+      </c>
+      <c r="M8" s="8">
+        <v>7.28</v>
+      </c>
       <c r="N8" s="3">
         <v>9.8000000000000007</v>
       </c>
@@ -1827,6 +2488,15 @@
       </c>
       <c r="P8" s="3">
         <v>9.85</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>12.09</v>
+      </c>
+      <c r="R8" s="8">
+        <v>12.09</v>
+      </c>
+      <c r="S8" s="8">
+        <v>12.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0814 updata-including parameter-to-force plots, models for different n values
</commit_message>
<xml_diff>
--- a/PycharmCodes_xlsxFiles/var_diam_data18mm.xlsx
+++ b/PycharmCodes_xlsxFiles/var_diam_data18mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d89e7b822021c56/Documents/성균관대학교/LAB/skku_robotory/PycharmCodes_xlsxFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="506" documentId="8_{07F248D2-7856-40A1-9CC6-E90616BB21F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CC89298-BC55-419F-A839-FD3207399554}"/>
+  <xr:revisionPtr revIDLastSave="528" documentId="8_{07F248D2-7856-40A1-9CC6-E90616BB21F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D597F964-F164-4D09-A926-9158F531DA4A}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A802EB2F-1C16-4A1A-977F-EE60EBC50092}"/>
+    <workbookView xWindow="3168" yWindow="2508" windowWidth="17280" windowHeight="11484" xr2:uid="{A802EB2F-1C16-4A1A-977F-EE60EBC50092}"/>
   </bookViews>
   <sheets>
     <sheet name="dn" sheetId="1" r:id="rId1"/>
@@ -768,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC1814F-43B7-4DF4-857A-25F58CC7AECE}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1142,6 +1142,9 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="M9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>